<commit_message>
added flat data files
</commit_message>
<xml_diff>
--- a/Resources/fall2017data.xlsx
+++ b/Resources/fall2017data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2189,7 +2189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>